<commit_message>
Re-run of Output tables for Table 2 Change
</commit_message>
<xml_diff>
--- a/final-outputs/Table A Corporate.xlsx
+++ b/final-outputs/Table A Corporate.xlsx
@@ -1,26 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\international-tax-competitiveness-index\final-outputs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFC1E43-DFC0-4238-A24B-8C699E4EB3A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="212">
   <si>
     <t>country</t>
   </si>
@@ -295,6 +287,9 @@
     <t>10</t>
   </si>
   <si>
+    <t>No Limit, capped at 50% of taxable income for companies with revenue above 1 million Euros</t>
+  </si>
+  <si>
     <t>No Limit, capped at EUR 1 million plus 60% of taxable income</t>
   </si>
   <si>
@@ -328,6 +323,9 @@
     <t>4</t>
   </si>
   <si>
+    <t>No Limit, capped at 50% of taxable income</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
@@ -496,12 +494,12 @@
     <t>Inventory (Best Available)</t>
   </si>
   <si>
+    <t>LIFO</t>
+  </si>
+  <si>
     <t>Average Cost</t>
   </si>
   <si>
-    <t>LIFO</t>
-  </si>
-  <si>
     <t>FIFO</t>
   </si>
   <si>
@@ -650,21 +648,16 @@
   </si>
   <si>
     <t>13</t>
-  </si>
-  <si>
-    <t>No Limit, capped at 50% of taxable income</t>
-  </si>
-  <si>
-    <t>No Limit, capped at 50% of taxable income for companies with revenue above 1 million Euros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -676,7 +669,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="darkGray"/>
     </fill>
   </fills>
   <borders count="1">
@@ -694,328 +687,18 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1082,7 +765,7 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
@@ -1097,7 +780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1111,34 +794,34 @@
         <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="K3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="L3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="M3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1149,37 +832,37 @@
         <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="L4" t="s">
         <v>82</v>
       </c>
       <c r="M4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1190,37 +873,37 @@
         <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="L5" t="s">
         <v>82</v>
       </c>
       <c r="M5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1228,40 +911,40 @@
         <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G6" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H6" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I6" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K6" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="L6" t="s">
         <v>82</v>
       </c>
       <c r="M6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1269,40 +952,40 @@
         <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I7" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J7" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="L7" t="s">
         <v>82</v>
       </c>
       <c r="M7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1313,28 +996,28 @@
         <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I8" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J8" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="K8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="L8" t="s">
         <v>82</v>
@@ -1343,7 +1026,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1354,28 +1037,28 @@
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H9" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I9" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J9" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="K9" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="L9" t="s">
         <v>82</v>
@@ -1384,7 +1067,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1392,40 +1075,40 @@
         <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H10" t="s">
         <v>160</v>
       </c>
       <c r="I10" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J10" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="K10" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="L10" t="s">
         <v>79</v>
       </c>
       <c r="M10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1433,28 +1116,28 @@
         <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H11" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="I11" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J11" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K11" t="s">
         <v>88</v>
@@ -1463,10 +1146,10 @@
         <v>82</v>
       </c>
       <c r="M11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1474,40 +1157,40 @@
         <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I12" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J12" t="s">
         <v>168</v>
       </c>
       <c r="K12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="L12" t="s">
         <v>82</v>
       </c>
       <c r="M12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1518,37 +1201,37 @@
         <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>211</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G13" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H13" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I13" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J13" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="K13" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="L13" t="s">
         <v>82</v>
       </c>
       <c r="M13" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1556,40 +1239,40 @@
         <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F14" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G14" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I14" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J14" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K14" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="L14" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1600,37 +1283,37 @@
         <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F15" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H15" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I15" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J15" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="K15" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="L15" t="s">
         <v>82</v>
       </c>
       <c r="M15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1641,37 +1324,37 @@
         <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F16" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H16" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I16" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K16" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="L16" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1679,40 +1362,40 @@
         <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F17" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G17" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H17" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I17" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J17" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K17" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="L17" t="s">
         <v>82</v>
       </c>
       <c r="M17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1720,40 +1403,40 @@
         <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
         <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F18" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G18" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I18" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J18" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="K18" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="L18" t="s">
         <v>82</v>
       </c>
       <c r="M18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1764,37 +1447,37 @@
         <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="E19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H19" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I19" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J19" t="s">
         <v>168</v>
       </c>
       <c r="K19" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="L19" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M19" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1805,37 +1488,37 @@
         <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E20" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F20" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G20" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H20" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I20" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J20" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K20" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="L20" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M20" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1843,40 +1526,40 @@
         <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E21" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F21" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G21" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H21" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I21" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J21" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="L21" t="s">
         <v>79</v>
       </c>
       <c r="M21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1884,40 +1567,40 @@
         <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E22" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F22" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G22" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J22" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="K22" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="L22" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M22" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1925,31 +1608,31 @@
         <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="E23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I23" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J23" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K23" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="L23" t="s">
         <v>82</v>
@@ -1958,7 +1641,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1969,37 +1652,37 @@
         <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E24" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F24" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G24" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I24" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J24" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="K24" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="L24" t="s">
         <v>82</v>
       </c>
       <c r="M24" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -2010,37 +1693,37 @@
         <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E25" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F25" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G25" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H25" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I25" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J25" t="s">
         <v>168</v>
       </c>
       <c r="K25" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="L25" t="s">
         <v>88</v>
       </c>
       <c r="M25" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -2048,31 +1731,31 @@
         <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E26" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F26" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G26" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H26" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I26" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J26" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K26" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="L26" t="s">
         <v>82</v>
@@ -2081,7 +1764,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -2089,40 +1772,40 @@
         <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F27" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H27" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="L27" t="s">
         <v>82</v>
       </c>
       <c r="M27" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2136,34 +1819,34 @@
         <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F28" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G28" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H28" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I28" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J28" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K28" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="L28" t="s">
         <v>82</v>
       </c>
       <c r="M28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2174,28 +1857,28 @@
         <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F29" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G29" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H29" t="s">
         <v>160</v>
       </c>
       <c r="I29" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J29" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="K29" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="L29" t="s">
         <v>82</v>
@@ -2204,7 +1887,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2215,37 +1898,37 @@
         <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E30" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F30" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G30" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H30" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I30" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J30" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="K30" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="L30" t="s">
         <v>82</v>
       </c>
       <c r="M30" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2256,37 +1939,37 @@
         <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F31" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G31" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H31" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I31" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J31" t="s">
         <v>169</v>
       </c>
       <c r="K31" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L31" t="s">
         <v>82</v>
       </c>
       <c r="M31" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2297,37 +1980,37 @@
         <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F32" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G32" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H32" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I32" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J32" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="K32" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="L32" t="s">
         <v>82</v>
       </c>
       <c r="M32" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2338,37 +2021,37 @@
         <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>210</v>
+        <v>80</v>
       </c>
       <c r="E33" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F33" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G33" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H33" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I33" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J33" t="s">
         <v>168</v>
       </c>
       <c r="K33" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="L33" t="s">
         <v>82</v>
       </c>
       <c r="M33" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2376,40 +2059,40 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D34" t="s">
         <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F34" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G34" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H34" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I34" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J34" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="K34" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="L34" t="s">
         <v>82</v>
       </c>
       <c r="M34" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2417,40 +2100,40 @@
         <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="E35" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F35" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G35" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H35" t="s">
         <v>160</v>
       </c>
       <c r="I35" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J35" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K35" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="L35" t="s">
         <v>82</v>
       </c>
       <c r="M35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -2461,37 +2144,37 @@
         <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F36" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G36" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H36" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I36" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J36" t="s">
         <v>168</v>
       </c>
       <c r="K36" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="L36" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M36" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2499,40 +2182,40 @@
         <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D37" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="E37" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F37" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G37" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H37" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I37" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J37" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K37" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="L37" t="s">
         <v>82</v>
       </c>
       <c r="M37" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2540,81 +2223,81 @@
         <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D38" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E38" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F38" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G38" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H38" t="s">
         <v>160</v>
       </c>
       <c r="I38" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J38" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K38" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="L38" t="s">
         <v>82</v>
       </c>
       <c r="M38" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39" t="s">
         <v>50</v>
       </c>
       <c r="B39" t="s">
         <v>75</v>
       </c>
-      <c r="C39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" t="s">
-        <v>93</v>
+      <c r="C39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D39" t="e">
+        <v>#N/A</v>
       </c>
       <c r="E39" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F39" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G39" t="s">
-        <v>109</v>
-      </c>
-      <c r="H39" t="s">
-        <v>159</v>
+        <v>111</v>
+      </c>
+      <c r="H39" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I39" t="s">
-        <v>163</v>
-      </c>
-      <c r="J39" t="s">
-        <v>166</v>
+        <v>165</v>
+      </c>
+      <c r="J39" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K39" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="L39" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M39" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update to Output Tables code and re-run of output
</commit_message>
<xml_diff>
--- a/final-outputs/Table A Corporate.xlsx
+++ b/final-outputs/Table A Corporate.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="212">
   <si>
     <t>country</t>
   </si>
@@ -302,7 +302,7 @@
     <t>10, capped at 50% of taxable income</t>
   </si>
   <si>
-    <t>10, capped at 60% of taxable income for companies other than small and medium-sized enterprises.</t>
+    <t>10, capped at 60% of taxable income for companies other than small and medium-sized enterprises</t>
   </si>
   <si>
     <t>No Limit, capped at 70% of taxable income</t>
@@ -494,10 +494,10 @@
     <t>Inventory (Best Available)</t>
   </si>
   <si>
+    <t>Average Cost</t>
+  </si>
+  <si>
     <t>LIFO</t>
-  </si>
-  <si>
-    <t>Average Cost</t>
   </si>
   <si>
     <t>FIFO</t>
@@ -832,7 +832,7 @@
         <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
         <v>107</v>
@@ -873,7 +873,7 @@
         <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
         <v>108</v>
@@ -885,7 +885,7 @@
         <v>115</v>
       </c>
       <c r="H5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I5" t="s">
         <v>165</v>
@@ -911,10 +911,10 @@
         <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
         <v>109</v>
@@ -952,10 +952,10 @@
         <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
         <v>110</v>
@@ -967,7 +967,7 @@
         <v>152</v>
       </c>
       <c r="H7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I7" t="s">
         <v>165</v>
@@ -996,7 +996,7 @@
         <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s">
         <v>111</v>
@@ -1008,13 +1008,13 @@
         <v>153</v>
       </c>
       <c r="H8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I8" t="s">
         <v>165</v>
       </c>
       <c r="J8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K8" t="s">
         <v>177</v>
@@ -1037,7 +1037,7 @@
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" t="s">
         <v>112</v>
@@ -1049,7 +1049,7 @@
         <v>154</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I9" t="s">
         <v>165</v>
@@ -1075,10 +1075,10 @@
         <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
         <v>113</v>
@@ -1090,13 +1090,13 @@
         <v>108</v>
       </c>
       <c r="H10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I10" t="s">
         <v>165</v>
       </c>
       <c r="J10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K10" t="s">
         <v>179</v>
@@ -1116,10 +1116,10 @@
         <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
         <v>110</v>
@@ -1131,7 +1131,7 @@
         <v>110</v>
       </c>
       <c r="H11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I11" t="s">
         <v>165</v>
@@ -1157,10 +1157,10 @@
         <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E12" t="s">
         <v>113</v>
@@ -1172,13 +1172,13 @@
         <v>115</v>
       </c>
       <c r="H12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I12" t="s">
         <v>165</v>
       </c>
       <c r="J12" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K12" t="s">
         <v>180</v>
@@ -1201,7 +1201,7 @@
         <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" t="s">
         <v>114</v>
@@ -1219,7 +1219,7 @@
         <v>166</v>
       </c>
       <c r="J13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K13" t="s">
         <v>181</v>
@@ -1239,10 +1239,10 @@
         <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
         <v>115</v>
@@ -1254,13 +1254,13 @@
         <v>119</v>
       </c>
       <c r="H14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I14" t="s">
         <v>165</v>
       </c>
       <c r="J14" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K14" t="s">
         <v>182</v>
@@ -1283,7 +1283,7 @@
         <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E15" t="s">
         <v>115</v>
@@ -1324,7 +1324,7 @@
         <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
         <v>116</v>
@@ -1336,13 +1336,13 @@
         <v>119</v>
       </c>
       <c r="H16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I16" t="s">
         <v>166</v>
       </c>
       <c r="J16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K16" t="s">
         <v>184</v>
@@ -1362,10 +1362,10 @@
         <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E17" t="s">
         <v>117</v>
@@ -1377,7 +1377,7 @@
         <v>155</v>
       </c>
       <c r="H17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I17" t="s">
         <v>165</v>
@@ -1403,7 +1403,7 @@
         <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
         <v>80</v>
@@ -1418,13 +1418,13 @@
         <v>140</v>
       </c>
       <c r="H18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I18" t="s">
         <v>166</v>
       </c>
       <c r="J18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K18" t="s">
         <v>186</v>
@@ -1447,7 +1447,7 @@
         <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
         <v>119</v>
@@ -1465,7 +1465,7 @@
         <v>166</v>
       </c>
       <c r="J19" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K19" t="s">
         <v>187</v>
@@ -1488,7 +1488,7 @@
         <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E20" t="s">
         <v>120</v>
@@ -1526,10 +1526,10 @@
         <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
         <v>121</v>
@@ -1567,10 +1567,10 @@
         <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="E22" t="s">
         <v>122</v>
@@ -1582,13 +1582,13 @@
         <v>115</v>
       </c>
       <c r="H22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I22" t="s">
         <v>166</v>
       </c>
       <c r="J22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K22" t="s">
         <v>190</v>
@@ -1608,10 +1608,10 @@
         <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="E23" t="s">
         <v>110</v>
@@ -1623,13 +1623,13 @@
         <v>110</v>
       </c>
       <c r="H23" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I23" t="s">
         <v>165</v>
       </c>
       <c r="J23" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K23" t="s">
         <v>191</v>
@@ -1652,7 +1652,7 @@
         <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
         <v>123</v>
@@ -1664,13 +1664,13 @@
         <v>156</v>
       </c>
       <c r="H24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I24" t="s">
         <v>166</v>
       </c>
       <c r="J24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K24" t="s">
         <v>180</v>
@@ -1693,7 +1693,7 @@
         <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E25" t="s">
         <v>124</v>
@@ -1705,13 +1705,13 @@
         <v>119</v>
       </c>
       <c r="H25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I25" t="s">
         <v>166</v>
       </c>
       <c r="J25" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K25" t="s">
         <v>192</v>
@@ -1731,10 +1731,10 @@
         <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E26" t="s">
         <v>115</v>
@@ -1746,7 +1746,7 @@
         <v>115</v>
       </c>
       <c r="H26" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I26" t="s">
         <v>165</v>
@@ -1772,10 +1772,10 @@
         <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="E27" t="s">
         <v>125</v>
@@ -1828,7 +1828,7 @@
         <v>115</v>
       </c>
       <c r="H28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I28" t="s">
         <v>165</v>
@@ -1857,7 +1857,7 @@
         <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E29" t="s">
         <v>127</v>
@@ -1869,13 +1869,13 @@
         <v>115</v>
       </c>
       <c r="H29" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I29" t="s">
         <v>165</v>
       </c>
       <c r="J29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K29" t="s">
         <v>195</v>
@@ -1898,7 +1898,7 @@
         <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E30" t="s">
         <v>115</v>
@@ -1916,7 +1916,7 @@
         <v>166</v>
       </c>
       <c r="J30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K30" t="s">
         <v>196</v>
@@ -1939,7 +1939,7 @@
         <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E31" t="s">
         <v>128</v>
@@ -1951,13 +1951,13 @@
         <v>115</v>
       </c>
       <c r="H31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I31" t="s">
         <v>166</v>
       </c>
       <c r="J31" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="K31" t="s">
         <v>197</v>
@@ -1980,7 +1980,7 @@
         <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E32" t="s">
         <v>112</v>
@@ -1992,13 +1992,13 @@
         <v>119</v>
       </c>
       <c r="H32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I32" t="s">
         <v>166</v>
       </c>
       <c r="J32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K32" t="s">
         <v>174</v>
@@ -2021,7 +2021,7 @@
         <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="E33" t="s">
         <v>119</v>
@@ -2033,13 +2033,13 @@
         <v>115</v>
       </c>
       <c r="H33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I33" t="s">
         <v>165</v>
       </c>
       <c r="J33" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K33" t="s">
         <v>198</v>
@@ -2059,7 +2059,7 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
         <v>80</v>
@@ -2074,13 +2074,13 @@
         <v>115</v>
       </c>
       <c r="H34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I34" t="s">
         <v>166</v>
       </c>
       <c r="J34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K34" t="s">
         <v>199</v>
@@ -2100,10 +2100,10 @@
         <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="E35" t="s">
         <v>117</v>
@@ -2115,7 +2115,7 @@
         <v>117</v>
       </c>
       <c r="H35" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I35" t="s">
         <v>165</v>
@@ -2144,7 +2144,7 @@
         <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="E36" t="s">
         <v>117</v>
@@ -2162,7 +2162,7 @@
         <v>165</v>
       </c>
       <c r="J36" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K36" t="s">
         <v>201</v>
@@ -2182,10 +2182,10 @@
         <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D37" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="E37" t="s">
         <v>130</v>
@@ -2197,7 +2197,7 @@
         <v>158</v>
       </c>
       <c r="H37" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I37" t="s">
         <v>166</v>
@@ -2223,10 +2223,10 @@
         <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="E38" t="s">
         <v>131</v>
@@ -2238,7 +2238,7 @@
         <v>113</v>
       </c>
       <c r="H38" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I38" t="s">
         <v>166</v>
@@ -2263,11 +2263,11 @@
       <c r="B39" t="s">
         <v>75</v>
       </c>
-      <c r="C39" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D39" t="e">
-        <v>#N/A</v>
+      <c r="C39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" t="s">
+        <v>94</v>
       </c>
       <c r="E39" t="s">
         <v>110</v>
@@ -2278,14 +2278,14 @@
       <c r="G39" t="s">
         <v>111</v>
       </c>
-      <c r="H39" t="e">
-        <v>#N/A</v>
+      <c r="H39" t="s">
+        <v>161</v>
       </c>
       <c r="I39" t="s">
         <v>165</v>
       </c>
-      <c r="J39" t="e">
-        <v>#N/A</v>
+      <c r="J39" t="s">
+        <v>168</v>
       </c>
       <c r="K39" t="s">
         <v>203</v>

</xml_diff>